<commit_message>
Updated with FIPS and Crime Index
</commit_message>
<xml_diff>
--- a/Project1_AmazonSites.xlsx
+++ b/Project1_AmazonSites.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ind\Desktop\BootCamp\Project1\BC_Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36A9F62-8658-4ACF-9597-8EC4478A8985}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F7C734-6134-4CFD-B391-DC9FA9F59A76}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AmazonSites" sheetId="1" r:id="rId1"/>
     <sheet name="AmazonCities" sheetId="2" r:id="rId2"/>
     <sheet name="CensusFields" sheetId="3" r:id="rId3"/>
+    <sheet name="AmzonCities_Crime" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="209">
   <si>
     <t>City</t>
   </si>
@@ -129,84 +130,51 @@
     <t>Number of persons, age 16 or older, in the labor force.</t>
   </si>
   <si>
-    <t>employment_employed</t>
-  </si>
-  <si>
     <t>B23025_004E</t>
   </si>
   <si>
     <t>Number of employed, age 16 or older, in the civilian labor force.</t>
   </si>
   <si>
-    <t>employment_civilian_labor_force</t>
-  </si>
-  <si>
     <t>B23025_003E</t>
   </si>
   <si>
     <t>Number of persons, age 16 or older, in the civilian labor force</t>
   </si>
   <si>
-    <t>employment_female_management_occupations</t>
-  </si>
-  <si>
     <t>C24010_041E</t>
   </si>
   <si>
     <t>Number of employed Female 'Management occupations' for the civilian population age 16 and over</t>
   </si>
   <si>
-    <t>employment_male_management_occupations</t>
-  </si>
-  <si>
     <t>C24010_005E</t>
   </si>
   <si>
     <t>Number of employed male 'Management occupations' for the civilian population age 16 and over</t>
   </si>
   <si>
-    <t>education_associates</t>
-  </si>
-  <si>
     <t>B15003_021E</t>
   </si>
   <si>
     <t>The number of persons age 25 and over who hold an Associate's degree.</t>
   </si>
   <si>
-    <t>education_bachelors</t>
-  </si>
-  <si>
     <t>B15003_022E</t>
   </si>
   <si>
-    <t>education_doctorate</t>
-  </si>
-  <si>
     <t>B15003_025E</t>
   </si>
   <si>
-    <t>education_ged</t>
-  </si>
-  <si>
     <t>B15003_018E</t>
   </si>
   <si>
-    <t>education_high_school</t>
-  </si>
-  <si>
     <t>B15003_017E</t>
   </si>
   <si>
-    <t>education_masters</t>
-  </si>
-  <si>
     <t>B15003_023E</t>
   </si>
   <si>
-    <t>education_professional</t>
-  </si>
-  <si>
     <t>B15003_024E</t>
   </si>
   <si>
@@ -216,93 +184,54 @@
     <t>B01003_001E</t>
   </si>
   <si>
-    <t>Population_american_indian_alone</t>
-  </si>
-  <si>
     <t>B02001_004E</t>
   </si>
   <si>
-    <t>Population_asian_alone</t>
-  </si>
-  <si>
     <t>B02001_005E</t>
   </si>
   <si>
-    <t>Population_black_alone</t>
-  </si>
-  <si>
     <t>B02001_003E</t>
   </si>
   <si>
-    <t>Population_hispanic_origin</t>
-  </si>
-  <si>
     <t>B03001_003E</t>
   </si>
   <si>
-    <t>Population_native_hawaiian_alone</t>
-  </si>
-  <si>
     <t>B02001_006E</t>
   </si>
   <si>
-    <t>Population_other_alone</t>
-  </si>
-  <si>
     <t>B02001_007E</t>
   </si>
   <si>
-    <t>Population_two_or_more_races</t>
-  </si>
-  <si>
     <t>B02001_008E</t>
   </si>
   <si>
-    <t>Population_white_alone</t>
-  </si>
-  <si>
     <t>B02001_002E</t>
   </si>
   <si>
-    <t>Commute_time</t>
-  </si>
-  <si>
     <t>B08136_001E</t>
   </si>
   <si>
     <t>(Normalizable) Total time spent commuting (in minutes).</t>
   </si>
   <si>
-    <t>Commute_time_carpool</t>
-  </si>
-  <si>
     <t>B08136_004E</t>
   </si>
   <si>
     <t>(Normalizable) Time spent commuting (in minutes): Car, truck, or van - carpool.</t>
   </si>
   <si>
-    <t>Commute_time_other</t>
-  </si>
-  <si>
     <t>B08136_012E</t>
   </si>
   <si>
     <t>(Normalizable) Time spent commuting (in minutes): Taxicab, motorcycle, bicycle, or other means.</t>
   </si>
   <si>
-    <t>Commute_time_public_transport</t>
-  </si>
-  <si>
     <t>B08136_007E</t>
   </si>
   <si>
     <t>(Normalizable) Time spent commuting (in minutes): public transport (excluding taxis).</t>
   </si>
   <si>
-    <t>Commute_time_solo_automobile</t>
-  </si>
-  <si>
     <t>B08136_003E</t>
   </si>
   <si>
@@ -646,6 +575,81 @@
   </si>
   <si>
     <t>04000</t>
+  </si>
+  <si>
+    <t>Emp_Mgment_Occp_Male</t>
+  </si>
+  <si>
+    <t>Emp_Total</t>
+  </si>
+  <si>
+    <t>Emp_civilian_labor_force</t>
+  </si>
+  <si>
+    <t>Emp_Mgment_Occp_Female</t>
+  </si>
+  <si>
+    <t>Ed_Bachelors</t>
+  </si>
+  <si>
+    <t>Ed_Doctorate</t>
+  </si>
+  <si>
+    <t>Ed_GED</t>
+  </si>
+  <si>
+    <t>Ed_HighSchool</t>
+  </si>
+  <si>
+    <t>Ed_Masters</t>
+  </si>
+  <si>
+    <t>Ed_Professional</t>
+  </si>
+  <si>
+    <t>Population_Asian</t>
+  </si>
+  <si>
+    <t>Pop_American_Indian</t>
+  </si>
+  <si>
+    <t>Pop_Black</t>
+  </si>
+  <si>
+    <t>Pop_Hispanic_Origin</t>
+  </si>
+  <si>
+    <t>Pop_Native_Hawaiian</t>
+  </si>
+  <si>
+    <t>Pop_Other</t>
+  </si>
+  <si>
+    <t>Pop_two_or_more_races</t>
+  </si>
+  <si>
+    <t>Ed_Associates</t>
+  </si>
+  <si>
+    <t>Pop_White</t>
+  </si>
+  <si>
+    <t>Commute_Time_Carpool</t>
+  </si>
+  <si>
+    <t>Commute_Time</t>
+  </si>
+  <si>
+    <t>Commute_Time_Other</t>
+  </si>
+  <si>
+    <t>Commute_Time_Public_Transport</t>
+  </si>
+  <si>
+    <t>Commute_Time_Solo_Automobile</t>
+  </si>
+  <si>
+    <t>CrimeIndex</t>
   </si>
 </sst>
 </file>
@@ -1210,16 +1214,16 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>0</v>
@@ -1228,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
@@ -1237,27 +1241,27 @@
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="G2" s="4">
         <v>20170</v>
@@ -1272,22 +1276,22 @@
     </row>
     <row r="3" spans="1:10" ht="15">
       <c r="A3" s="1" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="G3" s="2">
         <v>22202</v>
@@ -1305,16 +1309,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>7</v>
@@ -1335,16 +1339,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>7</v>
@@ -1365,16 +1369,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>7</v>
@@ -1395,16 +1399,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>7</v>
@@ -1425,16 +1429,16 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>15</v>
@@ -1455,16 +1459,16 @@
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>15</v>
@@ -1485,16 +1489,16 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>15</v>
@@ -1515,13 +1519,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>10</v>
@@ -1530,7 +1534,7 @@
         <v>11</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="H11" s="4">
         <v>42.39</v>
@@ -1539,7 +1543,7 @@
         <v>-71</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15">
@@ -1547,13 +1551,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>10</v>
@@ -1562,7 +1566,7 @@
         <v>11</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="H12" s="4">
         <v>42.34</v>
@@ -1577,13 +1581,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>10</v>
@@ -1592,7 +1596,7 @@
         <v>11</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="H13" s="4">
         <v>42.35</v>
@@ -1607,13 +1611,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>10</v>
@@ -1622,7 +1626,7 @@
         <v>11</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="H14" s="4">
         <v>42.34</v>
@@ -1637,13 +1641,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>8</v>
@@ -1667,16 +1671,16 @@
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>9</v>
@@ -1697,16 +1701,16 @@
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>9</v>
@@ -1727,16 +1731,16 @@
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>9</v>
@@ -1757,13 +1761,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="E19" s="21" t="s">
         <v>12</v>
@@ -1787,13 +1791,13 @@
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="E20" s="21" t="s">
         <v>12</v>
@@ -1817,13 +1821,13 @@
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>12</v>
@@ -1847,13 +1851,13 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>12</v>
@@ -1877,13 +1881,13 @@
         <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="E23" s="21" t="s">
         <v>12</v>
@@ -1907,13 +1911,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="E24" s="21" t="s">
         <v>12</v>
@@ -1937,13 +1941,13 @@
         <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="E25" s="21" t="s">
         <v>12</v>
@@ -1967,13 +1971,13 @@
         <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="E26" s="21" t="s">
         <v>12</v>
@@ -1997,16 +2001,16 @@
         <v>17</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>18</v>
@@ -2027,16 +2031,16 @@
         <v>17</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>18</v>
@@ -2057,13 +2061,13 @@
         <v>17</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>17</v>
@@ -2087,13 +2091,13 @@
         <v>21</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>21</v>
@@ -2117,13 +2121,13 @@
         <v>21</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>21</v>
@@ -2147,13 +2151,13 @@
         <v>21</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="E32" s="19" t="s">
         <v>21</v>
@@ -2177,13 +2181,13 @@
         <v>21</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="E33" s="19" t="s">
         <v>21</v>
@@ -2207,13 +2211,13 @@
         <v>19</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="E34" s="14" t="s">
         <v>19</v>
@@ -2231,7 +2235,7 @@
         <v>-97.744399999999999</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15">
@@ -2239,13 +2243,13 @@
         <v>19</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="E35" s="14" t="s">
         <v>19</v>
@@ -2269,13 +2273,13 @@
         <v>19</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="E36" s="14" t="s">
         <v>19</v>
@@ -2299,13 +2303,13 @@
         <v>19</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="E37" s="14" t="s">
         <v>19</v>
@@ -2329,13 +2333,13 @@
         <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="E38" s="14" t="s">
         <v>19</v>
@@ -2359,13 +2363,13 @@
         <v>19</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="E39" s="14" t="s">
         <v>19</v>
@@ -2389,13 +2393,13 @@
         <v>19</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="E40" s="14" t="s">
         <v>19</v>
@@ -5307,7 +5311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -5387,7 +5391,7 @@
         <v>-71.059799999999996</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="F4" s="5">
         <v>25</v>
@@ -5468,7 +5472,7 @@
         <v>-97.743099999999998</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="F8" s="5">
         <v>48</v>
@@ -5488,7 +5492,7 @@
         <v>-84.388000000000005</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="F9" s="5">
         <v>13</v>
@@ -5504,7 +5508,7 @@
   <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -5585,13 +5589,13 @@
     </row>
     <row r="6" spans="1:26" ht="15">
       <c r="A6" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="C6" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -5619,13 +5623,13 @@
     </row>
     <row r="7" spans="1:26" ht="15">
       <c r="A7" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -5653,13 +5657,13 @@
     </row>
     <row r="8" spans="1:26" ht="14.25">
       <c r="A8" s="34" t="s">
-        <v>41</v>
+        <v>187</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -5687,13 +5691,13 @@
     </row>
     <row r="9" spans="1:26" ht="15">
       <c r="A9" s="32" t="s">
-        <v>44</v>
+        <v>184</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -5721,13 +5725,13 @@
     </row>
     <row r="10" spans="1:26" ht="15">
       <c r="A10" s="35" t="s">
-        <v>47</v>
+        <v>201</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -5755,10 +5759,10 @@
     </row>
     <row r="11" spans="1:26" ht="15">
       <c r="A11" s="35" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -5787,10 +5791,10 @@
     </row>
     <row r="12" spans="1:26" ht="15">
       <c r="A12" s="35" t="s">
-        <v>52</v>
+        <v>189</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -5819,10 +5823,10 @@
     </row>
     <row r="13" spans="1:26" ht="15">
       <c r="A13" s="35" t="s">
-        <v>54</v>
+        <v>190</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -5851,10 +5855,10 @@
     </row>
     <row r="14" spans="1:26" ht="15">
       <c r="A14" s="35" t="s">
-        <v>56</v>
+        <v>191</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -5883,10 +5887,10 @@
     </row>
     <row r="15" spans="1:26" ht="15">
       <c r="A15" s="35" t="s">
-        <v>58</v>
+        <v>192</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -5915,10 +5919,10 @@
     </row>
     <row r="16" spans="1:26" ht="15">
       <c r="A16" s="35" t="s">
-        <v>60</v>
+        <v>193</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -5947,10 +5951,10 @@
     </row>
     <row r="17" spans="1:26" ht="14.25">
       <c r="A17" s="37" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -5979,10 +5983,10 @@
     </row>
     <row r="18" spans="1:26" ht="12.75">
       <c r="A18" s="37" t="s">
-        <v>64</v>
+        <v>195</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -6011,10 +6015,10 @@
     </row>
     <row r="19" spans="1:26" ht="12.75">
       <c r="A19" s="37" t="s">
-        <v>66</v>
+        <v>194</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -6043,10 +6047,10 @@
     </row>
     <row r="20" spans="1:26" ht="12.75">
       <c r="A20" s="40" t="s">
-        <v>68</v>
+        <v>196</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -6075,10 +6079,10 @@
     </row>
     <row r="21" spans="1:26" ht="12.75">
       <c r="A21" s="37" t="s">
-        <v>70</v>
+        <v>197</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -6107,10 +6111,10 @@
     </row>
     <row r="22" spans="1:26" ht="12.75">
       <c r="A22" s="40" t="s">
-        <v>72</v>
+        <v>198</v>
       </c>
       <c r="B22" s="40" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -6139,10 +6143,10 @@
     </row>
     <row r="23" spans="1:26" ht="12.75">
       <c r="A23" s="39" t="s">
-        <v>74</v>
+        <v>199</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -6171,10 +6175,10 @@
     </row>
     <row r="24" spans="1:26" ht="12.75">
       <c r="A24" s="37" t="s">
-        <v>76</v>
+        <v>200</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -6203,10 +6207,10 @@
     </row>
     <row r="25" spans="1:26" ht="12.75">
       <c r="A25" s="40" t="s">
-        <v>78</v>
+        <v>202</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
@@ -6235,13 +6239,13 @@
     </row>
     <row r="26" spans="1:26" ht="12.75">
       <c r="A26" s="41" t="s">
-        <v>80</v>
+        <v>204</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
@@ -6269,13 +6273,13 @@
     </row>
     <row r="27" spans="1:26" ht="12.75">
       <c r="A27" s="41" t="s">
-        <v>83</v>
+        <v>203</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
@@ -6303,13 +6307,13 @@
     </row>
     <row r="28" spans="1:26" ht="12.75">
       <c r="A28" s="41" t="s">
-        <v>86</v>
+        <v>205</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
@@ -6337,13 +6341,13 @@
     </row>
     <row r="29" spans="1:26" ht="12.75">
       <c r="A29" s="41" t="s">
-        <v>89</v>
+        <v>206</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
@@ -6371,13 +6375,13 @@
     </row>
     <row r="30" spans="1:26" ht="12.75">
       <c r="A30" s="41" t="s">
-        <v>92</v>
+        <v>207</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
@@ -6406,4 +6410,146 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1ED728-0DAC-462B-8BCA-D3A63DBEE251}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15">
+      <c r="A1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="26"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="15">
+      <c r="A2" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3">
+        <v>568.9</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" ht="15">
+      <c r="A3" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4">
+        <v>222.2</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" ht="15">
+      <c r="A4" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4">
+        <v>303.5</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" ht="15">
+      <c r="A5" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4">
+        <v>510.7</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" ht="15">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4">
+        <v>347.1</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="15">
+      <c r="A7" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4">
+        <v>259.8</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" ht="15">
+      <c r="A8" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4">
+        <v>312.7</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" ht="15">
+      <c r="A9" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4">
+        <v>591.79999999999995</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed the State and Place Codes
</commit_message>
<xml_diff>
--- a/Project1_AmazonSites.xlsx
+++ b/Project1_AmazonSites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ind\Desktop\BootCamp\Project1\BC_Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F7C734-6134-4CFD-B391-DC9FA9F59A76}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFE89B2-81BF-4C20-9A80-B7150E47FCC2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5550" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AmazonSites" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="210">
   <si>
     <t>City</t>
   </si>
@@ -650,6 +650,9 @@
   </si>
   <si>
     <t>CrimeIndex</t>
+  </si>
+  <si>
+    <t>50000</t>
   </si>
 </sst>
 </file>
@@ -5311,8 +5314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -5350,8 +5353,8 @@
       <c r="D2" s="3">
         <v>-77.016400000000004</v>
       </c>
-      <c r="E2" s="5">
-        <v>50000</v>
+      <c r="E2" s="5" t="s">
+        <v>209</v>
       </c>
       <c r="F2" s="5">
         <v>11</v>
@@ -5500,6 +5503,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2:F9" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -6416,7 +6423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1ED728-0DAC-462B-8BCA-D3A63DBEE251}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added Labor Force in Tech Occupations
</commit_message>
<xml_diff>
--- a/Project1_AmazonSites.xlsx
+++ b/Project1_AmazonSites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ind\Desktop\BootCamp\Project1\BC_Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFE89B2-81BF-4C20-9A80-B7150E47FCC2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BEDCB1-BCDF-4D17-BB46-6ECB3D4BCAAB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5550" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6660" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AmazonSites" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="217">
   <si>
     <t>City</t>
   </si>
@@ -142,18 +142,6 @@
     <t>Number of persons, age 16 or older, in the civilian labor force</t>
   </si>
   <si>
-    <t>C24010_041E</t>
-  </si>
-  <si>
-    <t>Number of employed Female 'Management occupations' for the civilian population age 16 and over</t>
-  </si>
-  <si>
-    <t>C24010_005E</t>
-  </si>
-  <si>
-    <t>Number of employed male 'Management occupations' for the civilian population age 16 and over</t>
-  </si>
-  <si>
     <t>B15003_021E</t>
   </si>
   <si>
@@ -653,13 +641,46 @@
   </si>
   <si>
     <t>50000</t>
+  </si>
+  <si>
+    <t>Median Household Income</t>
+  </si>
+  <si>
+    <t>B19013_001E</t>
+  </si>
+  <si>
+    <t>C24010_044E</t>
+  </si>
+  <si>
+    <t>Number of employed female 'Computer and mathematical occupations' for the civilian population age 16 and over</t>
+  </si>
+  <si>
+    <t>Emp_Comp_Math_Female</t>
+  </si>
+  <si>
+    <t>Number of employed male 'Computer and mathematical occupations' for the civilian population age 16 and over</t>
+  </si>
+  <si>
+    <t>C24010_008E</t>
+  </si>
+  <si>
+    <t>C24010_040E</t>
+  </si>
+  <si>
+    <t>Number of employed Female 'Management , Business and Financial occupations' for the civilian population age 16 and over</t>
+  </si>
+  <si>
+    <t>Number of employed male 'Management, Business and Financial  occupations' for the civilian population age 16 and over</t>
+  </si>
+  <si>
+    <t>C24010_006E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -716,6 +737,23 @@
     <font>
       <sz val="10"/>
       <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF31708F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Sans-serif"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF31708F"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -819,7 +857,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -884,12 +922,16 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1217,16 +1259,16 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>0</v>
@@ -1235,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
@@ -1244,27 +1286,27 @@
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15">
       <c r="A2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="G2" s="4">
         <v>20170</v>
@@ -1279,22 +1321,22 @@
     </row>
     <row r="3" spans="1:10" ht="15">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G3" s="2">
         <v>22202</v>
@@ -1312,16 +1354,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>7</v>
@@ -1342,16 +1384,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>7</v>
@@ -1372,16 +1414,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>7</v>
@@ -1402,16 +1444,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>7</v>
@@ -1432,16 +1474,16 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>15</v>
@@ -1462,16 +1504,16 @@
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>15</v>
@@ -1492,16 +1534,16 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>15</v>
@@ -1522,13 +1564,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>10</v>
@@ -1537,7 +1579,7 @@
         <v>11</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H11" s="4">
         <v>42.39</v>
@@ -1546,7 +1588,7 @@
         <v>-71</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15">
@@ -1554,13 +1596,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>10</v>
@@ -1569,7 +1611,7 @@
         <v>11</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H12" s="4">
         <v>42.34</v>
@@ -1584,13 +1626,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>10</v>
@@ -1599,7 +1641,7 @@
         <v>11</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H13" s="4">
         <v>42.35</v>
@@ -1614,13 +1656,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>10</v>
@@ -1629,7 +1671,7 @@
         <v>11</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H14" s="4">
         <v>42.34</v>
@@ -1644,13 +1686,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>8</v>
@@ -1674,16 +1716,16 @@
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>9</v>
@@ -1704,16 +1746,16 @@
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>9</v>
@@ -1734,16 +1776,16 @@
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>9</v>
@@ -1764,13 +1806,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E19" s="21" t="s">
         <v>12</v>
@@ -1794,13 +1836,13 @@
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E20" s="21" t="s">
         <v>12</v>
@@ -1824,13 +1866,13 @@
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>12</v>
@@ -1854,13 +1896,13 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>12</v>
@@ -1884,13 +1926,13 @@
         <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E23" s="21" t="s">
         <v>12</v>
@@ -1914,13 +1956,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E24" s="21" t="s">
         <v>12</v>
@@ -1944,13 +1986,13 @@
         <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E25" s="21" t="s">
         <v>12</v>
@@ -1974,13 +2016,13 @@
         <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E26" s="21" t="s">
         <v>12</v>
@@ -2004,16 +2046,16 @@
         <v>17</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>18</v>
@@ -2034,16 +2076,16 @@
         <v>17</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>18</v>
@@ -2064,13 +2106,13 @@
         <v>17</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>17</v>
@@ -2094,13 +2136,13 @@
         <v>21</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>21</v>
@@ -2124,13 +2166,13 @@
         <v>21</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>21</v>
@@ -2154,13 +2196,13 @@
         <v>21</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E32" s="19" t="s">
         <v>21</v>
@@ -2184,13 +2226,13 @@
         <v>21</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E33" s="19" t="s">
         <v>21</v>
@@ -2214,13 +2256,13 @@
         <v>19</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E34" s="14" t="s">
         <v>19</v>
@@ -2238,7 +2280,7 @@
         <v>-97.744399999999999</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15">
@@ -2246,13 +2288,13 @@
         <v>19</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E35" s="14" t="s">
         <v>19</v>
@@ -2276,13 +2318,13 @@
         <v>19</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E36" s="14" t="s">
         <v>19</v>
@@ -2306,13 +2348,13 @@
         <v>19</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E37" s="14" t="s">
         <v>19</v>
@@ -2336,13 +2378,13 @@
         <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E38" s="14" t="s">
         <v>19</v>
@@ -2366,13 +2408,13 @@
         <v>19</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E39" s="14" t="s">
         <v>19</v>
@@ -2396,13 +2438,13 @@
         <v>19</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E40" s="14" t="s">
         <v>19</v>
@@ -5314,7 +5356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -5354,7 +5396,7 @@
         <v>-77.016400000000004</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F2" s="5">
         <v>11</v>
@@ -5394,7 +5436,7 @@
         <v>-71.059799999999996</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F4" s="5">
         <v>25</v>
@@ -5475,7 +5517,7 @@
         <v>-97.743099999999998</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F8" s="5">
         <v>48</v>
@@ -5495,7 +5537,7 @@
         <v>-84.388000000000005</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F9" s="5">
         <v>13</v>
@@ -5512,17 +5554,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z30"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="52.85546875" customWidth="1"/>
+    <col min="1" max="1" width="66.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.42578125" customWidth="1"/>
-    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75">
@@ -5544,65 +5586,39 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25">
+    <row r="3" spans="1:26" ht="15">
       <c r="A3" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25">
+      <c r="A4" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B4" s="30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="12.75">
-      <c r="A4" s="29" t="s">
+    <row r="5" spans="1:26" ht="12.75">
+      <c r="A5" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B5" s="29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="16.5">
-      <c r="A5" s="31" t="s">
+    <row r="6" spans="1:26" ht="16.5">
+      <c r="A6" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B6" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C6" s="28" t="s">
         <v>34</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-    </row>
-    <row r="6" spans="1:26" ht="15">
-      <c r="A6" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -5630,13 +5646,13 @@
     </row>
     <row r="7" spans="1:26" ht="15">
       <c r="A7" s="32" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -5662,15 +5678,15 @@
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:26" ht="14.25">
-      <c r="A8" s="34" t="s">
-        <v>187</v>
+    <row r="8" spans="1:26" ht="15">
+      <c r="A8" s="32" t="s">
+        <v>182</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -5696,15 +5712,15 @@
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:26" ht="15">
-      <c r="A9" s="32" t="s">
-        <v>184</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>42</v>
+    <row r="9" spans="1:26">
+      <c r="A9" s="43" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>208</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>209</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -5730,112 +5746,118 @@
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
     </row>
-    <row r="10" spans="1:26" ht="15">
-      <c r="A10" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="B10" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
-    </row>
-    <row r="11" spans="1:26" ht="15">
-      <c r="A11" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="10"/>
-      <c r="Y11" s="10"/>
-      <c r="Z11" s="10"/>
+    <row r="10" spans="1:26" ht="14.25">
+      <c r="A10" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" s="43" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>212</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>211</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
     </row>
     <row r="12" spans="1:26" ht="15">
-      <c r="A12" s="35" t="s">
-        <v>189</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="10"/>
-      <c r="Y12" s="10"/>
-      <c r="Z12" s="10"/>
+      <c r="A12" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
     </row>
     <row r="13" spans="1:26" ht="15">
       <c r="A13" s="35" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="10"/>
+        <v>39</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -5862,10 +5884,10 @@
     </row>
     <row r="14" spans="1:26" ht="15">
       <c r="A14" s="35" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -5894,10 +5916,10 @@
     </row>
     <row r="15" spans="1:26" ht="15">
       <c r="A15" s="35" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -5926,10 +5948,10 @@
     </row>
     <row r="16" spans="1:26" ht="15">
       <c r="A16" s="35" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -5956,108 +5978,108 @@
       <c r="Y16" s="10"/>
       <c r="Z16" s="10"/>
     </row>
-    <row r="17" spans="1:26" ht="14.25">
-      <c r="A17" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
-    </row>
-    <row r="18" spans="1:26" ht="12.75">
-      <c r="A18" s="37" t="s">
-        <v>195</v>
-      </c>
-      <c r="B18" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="11"/>
-      <c r="T18" s="11"/>
-      <c r="U18" s="11"/>
-      <c r="V18" s="11"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
-    </row>
-    <row r="19" spans="1:26" ht="12.75">
-      <c r="A19" s="37" t="s">
-        <v>194</v>
-      </c>
-      <c r="B19" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="11"/>
-      <c r="W19" s="11"/>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="11"/>
-      <c r="Z19" s="11"/>
-    </row>
-    <row r="20" spans="1:26" ht="12.75">
-      <c r="A20" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="B20" s="40" t="s">
-        <v>55</v>
+    <row r="17" spans="1:26" ht="15">
+      <c r="A17" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+    </row>
+    <row r="18" spans="1:26" ht="15">
+      <c r="A18" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+    </row>
+    <row r="19" spans="1:26" ht="15">
+      <c r="A19" s="35" t="s">
+        <v>189</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+    </row>
+    <row r="20" spans="1:26" ht="14.25">
+      <c r="A20" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>48</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -6086,10 +6108,10 @@
     </row>
     <row r="21" spans="1:26" ht="12.75">
       <c r="A21" s="37" t="s">
-        <v>197</v>
-      </c>
-      <c r="B21" s="37" t="s">
-        <v>56</v>
+        <v>191</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>49</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -6117,11 +6139,11 @@
       <c r="Z21" s="11"/>
     </row>
     <row r="22" spans="1:26" ht="12.75">
-      <c r="A22" s="40" t="s">
-        <v>198</v>
-      </c>
-      <c r="B22" s="40" t="s">
-        <v>57</v>
+      <c r="A22" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>50</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -6150,10 +6172,10 @@
     </row>
     <row r="23" spans="1:26" ht="12.75">
       <c r="A23" s="39" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -6182,10 +6204,10 @@
     </row>
     <row r="24" spans="1:26" ht="12.75">
       <c r="A24" s="37" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -6213,11 +6235,11 @@
       <c r="Z24" s="11"/>
     </row>
     <row r="25" spans="1:26" ht="12.75">
-      <c r="A25" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="B25" s="40" t="s">
-        <v>60</v>
+      <c r="A25" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>53</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
@@ -6245,116 +6267,110 @@
       <c r="Z25" s="11"/>
     </row>
     <row r="26" spans="1:26" ht="12.75">
-      <c r="A26" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="B26" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
-      <c r="U26" s="13"/>
-      <c r="V26" s="13"/>
-      <c r="W26" s="13"/>
-      <c r="X26" s="13"/>
-      <c r="Y26" s="13"/>
-      <c r="Z26" s="13"/>
+      <c r="A26" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="11"/>
     </row>
     <row r="27" spans="1:26" ht="12.75">
-      <c r="A27" s="41" t="s">
-        <v>203</v>
-      </c>
-      <c r="B27" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="13"/>
-      <c r="V27" s="13"/>
-      <c r="W27" s="13"/>
-      <c r="X27" s="13"/>
-      <c r="Y27" s="13"/>
-      <c r="Z27" s="13"/>
+      <c r="A27" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="11"/>
+      <c r="Y27" s="11"/>
+      <c r="Z27" s="11"/>
     </row>
     <row r="28" spans="1:26" ht="12.75">
-      <c r="A28" s="41" t="s">
-        <v>205</v>
-      </c>
-      <c r="B28" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13"/>
-      <c r="U28" s="13"/>
-      <c r="V28" s="13"/>
-      <c r="W28" s="13"/>
-      <c r="X28" s="13"/>
-      <c r="Y28" s="13"/>
-      <c r="Z28" s="13"/>
+      <c r="A28" s="39" t="s">
+        <v>198</v>
+      </c>
+      <c r="B28" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+      <c r="X28" s="11"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="11"/>
     </row>
     <row r="29" spans="1:26" ht="12.75">
-      <c r="A29" s="41" t="s">
-        <v>206</v>
-      </c>
-      <c r="B29" s="41" t="s">
-        <v>67</v>
+      <c r="A29" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>57</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
@@ -6381,14 +6397,14 @@
       <c r="Z29" s="13"/>
     </row>
     <row r="30" spans="1:26" ht="12.75">
-      <c r="A30" s="41" t="s">
-        <v>207</v>
-      </c>
-      <c r="B30" s="41" t="s">
-        <v>69</v>
+      <c r="A30" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>59</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
@@ -6414,8 +6430,111 @@
       <c r="Y30" s="13"/>
       <c r="Z30" s="13"/>
     </row>
+    <row r="31" spans="1:26" ht="12.75">
+      <c r="A31" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="13"/>
+      <c r="W31" s="13"/>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="13"/>
+      <c r="Z31" s="13"/>
+    </row>
+    <row r="32" spans="1:26" ht="12.75">
+      <c r="A32" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="B32" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
+      <c r="W32" s="13"/>
+      <c r="X32" s="13"/>
+      <c r="Y32" s="13"/>
+      <c r="Z32" s="13"/>
+    </row>
+    <row r="33" spans="1:26" ht="12.75">
+      <c r="A33" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="B33" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="13"/>
+      <c r="V33" s="13"/>
+      <c r="W33" s="13"/>
+      <c r="X33" s="13"/>
+      <c r="Y33" s="13"/>
+      <c r="Z33" s="13"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6437,7 +6556,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D1" s="26"/>
       <c r="E1" s="2"/>

</xml_diff>